<commit_message>
Refactorization of code and changes on DB/Excel
</commit_message>
<xml_diff>
--- a/History_wp.xlsx
+++ b/History_wp.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="History Of Their Wp  " sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="History Of Their Wp" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,18 +432,15 @@
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="17" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id</t>
+          <t>Session ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -453,32 +450,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>Start DateTime</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Hour</t>
+          <t>End DateTime</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Minutes</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Second</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Type_Connection</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Online Time</t>
+          <t>Time Connected (s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Almudena</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-04-09 19:49:56</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-04-09 19:50:01</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Almudena</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-04-09 19:49:25</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-04-09 19:49:48</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>23</t>
         </is>
       </c>
     </row>

</xml_diff>